<commit_message>
Updates more tables, and adds TDES MCT algos
</commit_message>
<xml_diff>
--- a/tools/SpecBook.xlsx
+++ b/tools/SpecBook.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ctc\Documents\ACVP Protocol Documentation\tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentation-ACVP\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7BEB8AF0-C546-4588-BD37-A7AE47D836B0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6169EC55-A431-470A-A704-C09EA085279D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7050" xr2:uid="{4A423B63-A7B8-4728-A188-1056F06A2A15}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7050" activeTab="1" xr2:uid="{4A423B63-A7B8-4728-A188-1056F06A2A15}"/>
   </bookViews>
   <sheets>
     <sheet name="Symmetric Registration" sheetId="1" r:id="rId1"/>
+    <sheet name="Symmetric Prompt Test Group" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="71">
   <si>
     <t>algorithm</t>
   </si>
@@ -223,6 +224,21 @@
   </si>
   <si>
     <t>Min: 0, Max: 65536, Increment: any</t>
+  </si>
+  <si>
+    <t>within domain</t>
+  </si>
+  <si>
+    <t>incremental</t>
+  </si>
+  <si>
+    <t>overflow</t>
+  </si>
+  <si>
+    <t>1, 2</t>
+  </si>
+  <si>
+    <t>saltLen</t>
   </si>
 </sst>
 </file>
@@ -576,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACB07B3C-5951-470E-AC11-4876B2F0E9E2}">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,7 +658,7 @@
         <v>62</v>
       </c>
       <c r="G2" t="str">
-        <f>_xlfn.CONCAT(E2,_xlfn.TEXTJOIN(_xlfn.CONCAT(F2,E2),FALSE,A2:D2),F2)</f>
+        <f t="shared" ref="G2:G18" si="0">_xlfn.CONCAT(E2,_xlfn.TEXTJOIN(_xlfn.CONCAT(F2,E2),FALSE,A2:D2),F2)</f>
         <v>&lt;c&gt;AES-ECB&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
       </c>
     </row>
@@ -663,7 +679,7 @@
         <v>62</v>
       </c>
       <c r="G3" t="str">
-        <f>_xlfn.CONCAT(E3,_xlfn.TEXTJOIN(_xlfn.CONCAT(F3,E3),FALSE,A3:D3),F3)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;AES-CBC&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
       </c>
     </row>
@@ -684,7 +700,7 @@
         <v>62</v>
       </c>
       <c r="G4" t="str">
-        <f>_xlfn.CONCAT(E4,_xlfn.TEXTJOIN(_xlfn.CONCAT(F4,E4),FALSE,A4:D4),F4)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;AES-OFB&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
       </c>
     </row>
@@ -705,7 +721,7 @@
         <v>62</v>
       </c>
       <c r="G5" t="str">
-        <f>_xlfn.CONCAT(E5,_xlfn.TEXTJOIN(_xlfn.CONCAT(F5,E5),FALSE,A5:D5),F5)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;AES-CFB1&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
       </c>
     </row>
@@ -726,7 +742,7 @@
         <v>62</v>
       </c>
       <c r="G6" t="str">
-        <f>_xlfn.CONCAT(E6,_xlfn.TEXTJOIN(_xlfn.CONCAT(F6,E6),FALSE,A6:D6),F6)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;AES-CFB8&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
       </c>
     </row>
@@ -747,7 +763,7 @@
         <v>62</v>
       </c>
       <c r="G7" t="str">
-        <f>_xlfn.CONCAT(E7,_xlfn.TEXTJOIN(_xlfn.CONCAT(F7,E7),FALSE,A7:D7),F7)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;AES-CFB128&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
       </c>
     </row>
@@ -768,7 +784,7 @@
         <v>62</v>
       </c>
       <c r="G8" t="str">
-        <f>_xlfn.CONCAT(E8,_xlfn.TEXTJOIN(_xlfn.CONCAT(F8,E8),FALSE,A8:D8),F8)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;TDES-ECB&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2 Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
       </c>
     </row>
@@ -789,7 +805,7 @@
         <v>62</v>
       </c>
       <c r="G9" t="str">
-        <f>_xlfn.CONCAT(E9,_xlfn.TEXTJOIN(_xlfn.CONCAT(F9,E9),FALSE,A9:D9),F9)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;TDES-CBC&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2 Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
       </c>
     </row>
@@ -810,7 +826,7 @@
         <v>62</v>
       </c>
       <c r="G10" t="str">
-        <f>_xlfn.CONCAT(E10,_xlfn.TEXTJOIN(_xlfn.CONCAT(F10,E10),FALSE,A10:D10),F10)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;TDES-CBCI&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2 Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
       </c>
     </row>
@@ -831,7 +847,7 @@
         <v>62</v>
       </c>
       <c r="G11" t="str">
-        <f>_xlfn.CONCAT(E11,_xlfn.TEXTJOIN(_xlfn.CONCAT(F11,E11),FALSE,A11:D11),F11)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;TDES-CFB1&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2 Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
       </c>
     </row>
@@ -852,7 +868,7 @@
         <v>62</v>
       </c>
       <c r="G12" t="str">
-        <f>_xlfn.CONCAT(E12,_xlfn.TEXTJOIN(_xlfn.CONCAT(F12,E12),FALSE,A12:D12),F12)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;TDES-CFB8&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2 Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
       </c>
     </row>
@@ -873,7 +889,7 @@
         <v>62</v>
       </c>
       <c r="G13" t="str">
-        <f>_xlfn.CONCAT(E13,_xlfn.TEXTJOIN(_xlfn.CONCAT(F13,E13),FALSE,A13:D13),F13)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;TDES-CFB64&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2 Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
       </c>
     </row>
@@ -894,7 +910,7 @@
         <v>62</v>
       </c>
       <c r="G14" t="str">
-        <f>_xlfn.CONCAT(E14,_xlfn.TEXTJOIN(_xlfn.CONCAT(F14,E14),FALSE,A14:D14),F14)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;TDES-CFBP1&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2 Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
       </c>
     </row>
@@ -915,7 +931,7 @@
         <v>62</v>
       </c>
       <c r="G15" t="str">
-        <f>_xlfn.CONCAT(E15,_xlfn.TEXTJOIN(_xlfn.CONCAT(F15,E15),FALSE,A15:D15),F15)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;TDES-CFBP8&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2 Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
       </c>
     </row>
@@ -936,7 +952,7 @@
         <v>62</v>
       </c>
       <c r="G16" t="str">
-        <f>_xlfn.CONCAT(E16,_xlfn.TEXTJOIN(_xlfn.CONCAT(F16,E16),FALSE,A16:D16),F16)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;TDES-CFBP64&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2 Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
       </c>
     </row>
@@ -957,7 +973,7 @@
         <v>62</v>
       </c>
       <c r="G17" t="str">
-        <f>_xlfn.CONCAT(E17,_xlfn.TEXTJOIN(_xlfn.CONCAT(F17,E17),FALSE,A17:D17),F17)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;TDES-OFB&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2 Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
       </c>
     </row>
@@ -978,7 +994,7 @@
         <v>62</v>
       </c>
       <c r="G18" t="str">
-        <f>_xlfn.CONCAT(E18,_xlfn.TEXTJOIN(_xlfn.CONCAT(F18,E18),FALSE,A18:D18),F18)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;TDES-OFBI&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2 Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
       </c>
     </row>
@@ -1358,6 +1374,711 @@
       <c r="K39" t="str">
         <f>_xlfn.CONCAT(I39,_xlfn.TEXTJOIN(_xlfn.CONCAT(J39,I39),FALSE,A39:H39),J39)</f>
         <v>&lt;c&gt;TDES-CTR&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;Min: 1, Max: 64, Increment: any&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2 Note: 2 is only available for decrypt operations&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4BEB1AA-8A6E-4317-A406-8B0373CC58E9}">
+  <dimension ref="A1:M39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" t="str">
+        <f>_xlfn.CONCAT(D1,_xlfn.TEXTJOIN(_xlfn.CONCAT(E1,D1),FALSE,A1:C1),E1)</f>
+        <v>&lt;ttcol align="left"&gt;algorithm&lt;/ttcol&gt;&lt;ttcol align="left"&gt;keyLen&lt;/ttcol&gt;&lt;ttcol align="left"&gt;keyingOption&lt;/ttcol&gt;</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" t="str">
+        <f>_xlfn.CONCAT(D2,_xlfn.TEXTJOIN(_xlfn.CONCAT(E2,D2),FALSE,A2:C2),E2)</f>
+        <v>&lt;c&gt;AES-ECB&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" t="str">
+        <f>_xlfn.CONCAT(D3,_xlfn.TEXTJOIN(_xlfn.CONCAT(E3,D3),FALSE,A3:C3),E3)</f>
+        <v>&lt;c&gt;AES-CBC&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" t="str">
+        <f>_xlfn.CONCAT(D4,_xlfn.TEXTJOIN(_xlfn.CONCAT(E4,D4),FALSE,A4:C4),E4)</f>
+        <v>&lt;c&gt;AES-OFB&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" t="str">
+        <f>_xlfn.CONCAT(D5,_xlfn.TEXTJOIN(_xlfn.CONCAT(E5,D5),FALSE,A5:C5),E5)</f>
+        <v>&lt;c&gt;AES-CFB1&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" t="str">
+        <f>_xlfn.CONCAT(D6,_xlfn.TEXTJOIN(_xlfn.CONCAT(E6,D6),FALSE,A6:C6),E6)</f>
+        <v>&lt;c&gt;AES-CFB8&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" t="str">
+        <f>_xlfn.CONCAT(D7,_xlfn.TEXTJOIN(_xlfn.CONCAT(E7,D7),FALSE,A7:C7),E7)</f>
+        <v>&lt;c&gt;AES-CFB128&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" t="str">
+        <f>_xlfn.CONCAT(D8,_xlfn.TEXTJOIN(_xlfn.CONCAT(E8,D8),FALSE,A8:C8),E8)</f>
+        <v>&lt;c&gt;TDES-ECB&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" t="str">
+        <f>_xlfn.CONCAT(D9,_xlfn.TEXTJOIN(_xlfn.CONCAT(E9,D9),FALSE,A9:C9),E9)</f>
+        <v>&lt;c&gt;TDES-CBC&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" t="str">
+        <f>_xlfn.CONCAT(D10,_xlfn.TEXTJOIN(_xlfn.CONCAT(E10,D10),FALSE,A10:C10),E10)</f>
+        <v>&lt;c&gt;TDES-CBCI&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" t="str">
+        <f>_xlfn.CONCAT(D11,_xlfn.TEXTJOIN(_xlfn.CONCAT(E11,D11),FALSE,A11:C11),E11)</f>
+        <v>&lt;c&gt;TDES-CFB1&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" t="str">
+        <f>_xlfn.CONCAT(D12,_xlfn.TEXTJOIN(_xlfn.CONCAT(E12,D12),FALSE,A12:C12),E12)</f>
+        <v>&lt;c&gt;TDES-CFB8&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" t="str">
+        <f>_xlfn.CONCAT(D13,_xlfn.TEXTJOIN(_xlfn.CONCAT(E13,D13),FALSE,A13:C13),E13)</f>
+        <v>&lt;c&gt;TDES-CFB64&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" t="str">
+        <f>_xlfn.CONCAT(D14,_xlfn.TEXTJOIN(_xlfn.CONCAT(E14,D14),FALSE,A14:C14),E14)</f>
+        <v>&lt;c&gt;TDES-CFBP1&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" t="str">
+        <f>_xlfn.CONCAT(D15,_xlfn.TEXTJOIN(_xlfn.CONCAT(E15,D15),FALSE,A15:C15),E15)</f>
+        <v>&lt;c&gt;TDES-CFBP8&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" t="str">
+        <f>_xlfn.CONCAT(D16,_xlfn.TEXTJOIN(_xlfn.CONCAT(E16,D16),FALSE,A16:C16),E16)</f>
+        <v>&lt;c&gt;TDES-CFBP64&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" t="str">
+        <f>_xlfn.CONCAT(D17,_xlfn.TEXTJOIN(_xlfn.CONCAT(E17,D17),FALSE,A17:C17),E17)</f>
+        <v>&lt;c&gt;TDES-OFB&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" t="str">
+        <f>_xlfn.CONCAT(D18,_xlfn.TEXTJOIN(_xlfn.CONCAT(E18,D18),FALSE,A18:C18),E18)</f>
+        <v>&lt;c&gt;TDES-OFBI&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" t="s">
+        <v>59</v>
+      </c>
+      <c r="G22" t="s">
+        <v>60</v>
+      </c>
+      <c r="H22" t="str">
+        <f>_xlfn.CONCAT(F22,_xlfn.TEXTJOIN(_xlfn.CONCAT(G22,F22),FALSE,A22:E22),G22)</f>
+        <v>&lt;ttcol align="left"&gt;algorithm&lt;/ttcol&gt;&lt;ttcol align="left"&gt;keyLen&lt;/ttcol&gt;&lt;ttcol align="left"&gt;keyingOption&lt;/ttcol&gt;&lt;ttcol align="left"&gt;kwCipher&lt;/ttcol&gt;&lt;ttcol align="left"&gt;dataLen&lt;/ttcol&gt;</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" t="s">
+        <v>61</v>
+      </c>
+      <c r="G23" t="s">
+        <v>62</v>
+      </c>
+      <c r="H23" t="str">
+        <f>_xlfn.CONCAT(F23,_xlfn.TEXTJOIN(_xlfn.CONCAT(G23,F23),FALSE,A23:E23),G23)</f>
+        <v>&lt;c&gt;AES-KW&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;"cipher", "inverse"&lt;/c&gt;&lt;c&gt;within domain&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" t="s">
+        <v>66</v>
+      </c>
+      <c r="F24" t="s">
+        <v>61</v>
+      </c>
+      <c r="G24" t="s">
+        <v>62</v>
+      </c>
+      <c r="H24" t="str">
+        <f>_xlfn.CONCAT(F24,_xlfn.TEXTJOIN(_xlfn.CONCAT(G24,F24),FALSE,A24:E24),G24)</f>
+        <v>&lt;c&gt;AES-KWP&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;"cipher", "inverse"&lt;/c&gt;&lt;c&gt;within domain&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" t="s">
+        <v>66</v>
+      </c>
+      <c r="F25" t="s">
+        <v>61</v>
+      </c>
+      <c r="G25" t="s">
+        <v>62</v>
+      </c>
+      <c r="H25" t="str">
+        <f>_xlfn.CONCAT(F25,_xlfn.TEXTJOIN(_xlfn.CONCAT(G25,F25),FALSE,A25:E25),G25)</f>
+        <v>&lt;c&gt;TDES-KW&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2&lt;/c&gt;&lt;c&gt;"cipher", "inverse"&lt;/c&gt;&lt;c&gt;within domain&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" t="s">
+        <v>4</v>
+      </c>
+      <c r="G29" t="s">
+        <v>3</v>
+      </c>
+      <c r="H29" t="s">
+        <v>8</v>
+      </c>
+      <c r="I29" t="s">
+        <v>9</v>
+      </c>
+      <c r="J29" t="s">
+        <v>70</v>
+      </c>
+      <c r="K29" t="s">
+        <v>59</v>
+      </c>
+      <c r="L29" t="s">
+        <v>60</v>
+      </c>
+      <c r="M29" t="str">
+        <f>_xlfn.CONCAT(K29,_xlfn.TEXTJOIN(_xlfn.CONCAT(L29,K29),FALSE,A29:J29),L29)</f>
+        <v>&lt;ttcol align="left"&gt;algorithm&lt;/ttcol&gt;&lt;ttcol align="left"&gt;keyLen&lt;/ttcol&gt;&lt;ttcol align="left"&gt;ivGen&lt;/ttcol&gt;&lt;ttcol align="left"&gt;ivGenMode&lt;/ttcol&gt;&lt;ttcol align="left"&gt;saltGen&lt;/ttcol&gt;&lt;ttcol align="left"&gt;ivLen&lt;/ttcol&gt;&lt;ttcol align="left"&gt;dataLen&lt;/ttcol&gt;&lt;ttcol align="left"&gt;aadLen&lt;/ttcol&gt;&lt;ttcol align="left"&gt;tagLen&lt;/ttcol&gt;&lt;ttcol align="left"&gt;saltLen&lt;/ttcol&gt;</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" t="s">
+        <v>46</v>
+      </c>
+      <c r="F30" t="s">
+        <v>66</v>
+      </c>
+      <c r="G30" t="s">
+        <v>66</v>
+      </c>
+      <c r="H30" t="s">
+        <v>66</v>
+      </c>
+      <c r="I30" t="s">
+        <v>66</v>
+      </c>
+      <c r="K30" t="s">
+        <v>61</v>
+      </c>
+      <c r="L30" t="s">
+        <v>62</v>
+      </c>
+      <c r="M30" t="str">
+        <f>_xlfn.CONCAT(K30,_xlfn.TEXTJOIN(_xlfn.CONCAT(L30,K30),FALSE,A30:J30),L30)</f>
+        <v>&lt;c&gt;AES-GCM&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;"internal", "external"&lt;/c&gt;&lt;c&gt;"8.2.1", "8.2.2"&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;within domain&lt;/c&gt;&lt;c&gt;within domain&lt;/c&gt;&lt;c&gt;within domain&lt;/c&gt;&lt;c&gt;within domain&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" t="s">
+        <v>45</v>
+      </c>
+      <c r="F31" t="s">
+        <v>66</v>
+      </c>
+      <c r="G31" t="s">
+        <v>66</v>
+      </c>
+      <c r="H31" t="s">
+        <v>66</v>
+      </c>
+      <c r="I31" t="s">
+        <v>66</v>
+      </c>
+      <c r="J31" t="s">
+        <v>66</v>
+      </c>
+      <c r="K31" t="s">
+        <v>61</v>
+      </c>
+      <c r="L31" t="s">
+        <v>62</v>
+      </c>
+      <c r="M31" t="str">
+        <f>_xlfn.CONCAT(K31,_xlfn.TEXTJOIN(_xlfn.CONCAT(L31,K31),FALSE,A31:J31),L31)</f>
+        <v>&lt;c&gt;AES-XPN&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;"internal", "external"&lt;/c&gt;&lt;c&gt;"8.2.1", "8.2.2"&lt;/c&gt;&lt;c&gt;"internal", "external"&lt;/c&gt;&lt;c&gt;within domain&lt;/c&gt;&lt;c&gt;within domain&lt;/c&gt;&lt;c&gt;within domain&lt;/c&gt;&lt;c&gt;within domain&lt;/c&gt;&lt;c&gt;within domain&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" t="s">
+        <v>40</v>
+      </c>
+      <c r="F32" t="s">
+        <v>66</v>
+      </c>
+      <c r="G32" t="s">
+        <v>66</v>
+      </c>
+      <c r="H32" t="s">
+        <v>66</v>
+      </c>
+      <c r="I32" t="s">
+        <v>66</v>
+      </c>
+      <c r="K32" t="s">
+        <v>61</v>
+      </c>
+      <c r="L32" t="s">
+        <v>62</v>
+      </c>
+      <c r="M32" t="str">
+        <f>_xlfn.CONCAT(K32,_xlfn.TEXTJOIN(_xlfn.CONCAT(L32,K32),FALSE,A32:J32),L32)</f>
+        <v>&lt;c&gt;AES-CCM&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;within domain&lt;/c&gt;&lt;c&gt;within domain&lt;/c&gt;&lt;c&gt;within domain&lt;/c&gt;&lt;c&gt;within domain&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" t="s">
+        <v>67</v>
+      </c>
+      <c r="E36" t="s">
+        <v>68</v>
+      </c>
+      <c r="F36" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" t="s">
+        <v>3</v>
+      </c>
+      <c r="H36" t="s">
+        <v>59</v>
+      </c>
+      <c r="I36" t="s">
+        <v>60</v>
+      </c>
+      <c r="J36" t="str">
+        <f>_xlfn.CONCAT(H36,_xlfn.TEXTJOIN(_xlfn.CONCAT(I36,H36),FALSE,A36:G36),I36)</f>
+        <v>&lt;ttcol align="left"&gt;algorithm&lt;/ttcol&gt;&lt;ttcol align="left"&gt;keyLen&lt;/ttcol&gt;&lt;ttcol align="left"&gt;keyingOption&lt;/ttcol&gt;&lt;ttcol align="left"&gt;incremental&lt;/ttcol&gt;&lt;ttcol align="left"&gt;overflow&lt;/ttcol&gt;&lt;ttcol align="left"&gt;tweakMode&lt;/ttcol&gt;&lt;ttcol align="left"&gt;dataLen&lt;/ttcol&gt;</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" t="s">
+        <v>42</v>
+      </c>
+      <c r="E37" t="s">
+        <v>42</v>
+      </c>
+      <c r="H37" t="s">
+        <v>61</v>
+      </c>
+      <c r="I37" t="s">
+        <v>62</v>
+      </c>
+      <c r="J37" t="str">
+        <f>_xlfn.CONCAT(H37,_xlfn.TEXTJOIN(_xlfn.CONCAT(I37,H37),FALSE,A37:G37),I37)</f>
+        <v>&lt;c&gt;AES-CTR&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" t="s">
+        <v>41</v>
+      </c>
+      <c r="F38" t="s">
+        <v>44</v>
+      </c>
+      <c r="G38" t="s">
+        <v>66</v>
+      </c>
+      <c r="H38" t="s">
+        <v>61</v>
+      </c>
+      <c r="I38" t="s">
+        <v>62</v>
+      </c>
+      <c r="J38" t="str">
+        <f>_xlfn.CONCAT(H38,_xlfn.TEXTJOIN(_xlfn.CONCAT(I38,H38),FALSE,A38:G38),I38)</f>
+        <v>&lt;c&gt;AES-XTS&lt;/c&gt;&lt;c&gt;128, 256&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;"hex", "number"&lt;/c&gt;&lt;c&gt;within domain&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" t="s">
+        <v>69</v>
+      </c>
+      <c r="D39" t="s">
+        <v>42</v>
+      </c>
+      <c r="E39" t="s">
+        <v>42</v>
+      </c>
+      <c r="H39" t="s">
+        <v>61</v>
+      </c>
+      <c r="I39" t="s">
+        <v>62</v>
+      </c>
+      <c r="J39" t="str">
+        <f>_xlfn.CONCAT(H39,_xlfn.TEXTJOIN(_xlfn.CONCAT(I39,H39),FALSE,A39:G39),I39)</f>
+        <v>&lt;c&gt;TDES-CTR&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moves Test Types and coverage section up to the front. Fixes tables to include [] {} around arrays and objects
</commit_message>
<xml_diff>
--- a/tools/SpecBook.xlsx
+++ b/tools/SpecBook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentation-ACVP\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6169EC55-A431-470A-A704-C09EA085279D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{94F91522-14C5-4208-8440-478E1BEC7FAB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7050" activeTab="1" xr2:uid="{4A423B63-A7B8-4728-A188-1056F06A2A15}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="78">
   <si>
     <t>algorithm</t>
   </si>
@@ -145,9 +145,6 @@
     <t>TDES-KW</t>
   </si>
   <si>
-    <t>"encrypt", "decrypt"</t>
-  </si>
-  <si>
     <t>128, 192, 256</t>
   </si>
   <si>
@@ -172,39 +169,9 @@
     <t>AES-CCM</t>
   </si>
   <si>
-    <t>Min: 1, Max: 128, Increment: any</t>
-  </si>
-  <si>
-    <t>Min: 1, Max: 64, Increment: any</t>
-  </si>
-  <si>
     <t>"cipher", "inverse"</t>
   </si>
   <si>
-    <t>Min: 0, Max: 256, Increment: 8</t>
-  </si>
-  <si>
-    <t>Min: 1, Max: xxx, Increment: any</t>
-  </si>
-  <si>
-    <t>32, 64, 96, 104, 112, 120, 128</t>
-  </si>
-  <si>
-    <t>Min: 32, Max: 128, Increment: 16</t>
-  </si>
-  <si>
-    <t>Min: 8, Max: 1024, Increment: any</t>
-  </si>
-  <si>
-    <t>Min: 56, Max: 104, Increment: 8</t>
-  </si>
-  <si>
-    <t>Min: 0, Max: 524288, Increment: any</t>
-  </si>
-  <si>
-    <t>1, 2 Note: 2 is only available for decrypt operations</t>
-  </si>
-  <si>
     <t>&lt;ttcol align="left"&gt;</t>
   </si>
   <si>
@@ -217,15 +184,6 @@
     <t>&lt;/c&gt;</t>
   </si>
   <si>
-    <t>Min: 128, Max: 65536, Increment: 128</t>
-  </si>
-  <si>
-    <t>Min: 1, Max: any, Increment: any</t>
-  </si>
-  <si>
-    <t>Min: 0, Max: 65536, Increment: any</t>
-  </si>
-  <si>
     <t>within domain</t>
   </si>
   <si>
@@ -239,6 +197,69 @@
   </si>
   <si>
     <t>saltLen</t>
+  </si>
+  <si>
+    <t>[128, 192, 256]</t>
+  </si>
+  <si>
+    <t>["encrypt", "decrypt"]</t>
+  </si>
+  <si>
+    <t>[1, 2] Note: 2 is only available for decrypt operations</t>
+  </si>
+  <si>
+    <t>[128, 256]</t>
+  </si>
+  <si>
+    <t>["cipher", "inverse"]</t>
+  </si>
+  <si>
+    <t>{"Min": 0, "Max": 65536, "Inc": any}</t>
+  </si>
+  <si>
+    <t>{"Min": 1, "Max": xxx, "Inc": any}</t>
+  </si>
+  <si>
+    <t>{"Min": 0, "Max": 256, "Inc": 8}</t>
+  </si>
+  <si>
+    <t>{"Min": 128, "Max": 65536, "Inc": 128}</t>
+  </si>
+  <si>
+    <t>{"Min": 1, "Max": 64, "Inc": any}</t>
+  </si>
+  <si>
+    <t>["hex", "number"]</t>
+  </si>
+  <si>
+    <t>{"Min": 1, "Max": 128, "Inc": any}</t>
+  </si>
+  <si>
+    <t>{"Min": 8, Max: 1024, Increment: any</t>
+  </si>
+  <si>
+    <t>["internal", "external"]</t>
+  </si>
+  <si>
+    <t>["8.2.1", "8.2.2"]</t>
+  </si>
+  <si>
+    <t>{[32, 64, 96, 104, 112, 120, 128]}</t>
+  </si>
+  <si>
+    <t>{"Min": 8, "Max": 1024, "Inc": any}</t>
+  </si>
+  <si>
+    <t>{"Min": 56, "Max": 104, "Inc": 8}</t>
+  </si>
+  <si>
+    <t>{"Min": 1, "Max": any, "Inc": any}</t>
+  </si>
+  <si>
+    <t>{"Min": 0, "Max": 524288, "Inc": any}</t>
+  </si>
+  <si>
+    <t>{"Min": 32, "Max": 128, "Inc": 16}</t>
   </si>
 </sst>
 </file>
@@ -593,15 +614,15 @@
   <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:G2"/>
+      <selection activeCell="M29" sqref="M29:M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
@@ -631,10 +652,10 @@
         <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="F1" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="G1" t="str">
         <f>_xlfn.CONCAT(E1,_xlfn.TEXTJOIN(_xlfn.CONCAT(F1,E1),,A1:D1),F1)</f>
@@ -646,20 +667,20 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="G2" t="str">
         <f t="shared" ref="G2:G18" si="0">_xlfn.CONCAT(E2,_xlfn.TEXTJOIN(_xlfn.CONCAT(F2,E2),FALSE,A2:D2),F2)</f>
-        <v>&lt;c&gt;AES-ECB&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
+        <v>&lt;c&gt;AES-ECB&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -667,20 +688,20 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F3" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;c&gt;AES-CBC&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
+        <v>&lt;c&gt;AES-CBC&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -688,20 +709,20 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F4" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;c&gt;AES-OFB&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
+        <v>&lt;c&gt;AES-OFB&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -709,20 +730,20 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F5" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;c&gt;AES-CFB1&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
+        <v>&lt;c&gt;AES-CFB1&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -730,20 +751,20 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="E6" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F6" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;c&gt;AES-CFB8&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
+        <v>&lt;c&gt;AES-CFB8&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -751,20 +772,20 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="E7" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F7" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;c&gt;AES-CFB128&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
+        <v>&lt;c&gt;AES-CFB128&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -772,20 +793,20 @@
         <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E8" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F8" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;c&gt;TDES-ECB&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2 Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
+        <v>&lt;c&gt;TDES-ECB&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -793,20 +814,20 @@
         <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E9" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F9" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;c&gt;TDES-CBC&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2 Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
+        <v>&lt;c&gt;TDES-CBC&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -814,20 +835,20 @@
         <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="D10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E10" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;c&gt;TDES-CBCI&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2 Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
+        <v>&lt;c&gt;TDES-CBCI&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -835,20 +856,20 @@
         <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E11" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F11" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;c&gt;TDES-CFB1&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2 Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
+        <v>&lt;c&gt;TDES-CFB1&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -856,20 +877,20 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E12" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F12" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;c&gt;TDES-CFB8&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2 Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
+        <v>&lt;c&gt;TDES-CFB8&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -877,20 +898,20 @@
         <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="D13" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E13" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F13" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;c&gt;TDES-CFB64&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2 Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
+        <v>&lt;c&gt;TDES-CFB64&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -898,20 +919,20 @@
         <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="D14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E14" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F14" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;c&gt;TDES-CFBP1&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2 Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
+        <v>&lt;c&gt;TDES-CFBP1&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -919,20 +940,20 @@
         <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E15" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F15" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;c&gt;TDES-CFBP8&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2 Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
+        <v>&lt;c&gt;TDES-CFBP8&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -940,20 +961,20 @@
         <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="D16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E16" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F16" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;c&gt;TDES-CFBP64&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2 Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
+        <v>&lt;c&gt;TDES-CFBP64&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -961,20 +982,20 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="D17" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E17" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F17" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;c&gt;TDES-OFB&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2 Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
+        <v>&lt;c&gt;TDES-OFB&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -982,20 +1003,20 @@
         <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E18" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F18" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;c&gt;TDES-OFBI&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2 Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
+        <v>&lt;c&gt;TDES-OFBI&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -1015,10 +1036,10 @@
         <v>12</v>
       </c>
       <c r="F22" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="G22" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="H22" t="str">
         <f>_xlfn.CONCAT(F22,_xlfn.TEXTJOIN(_xlfn.CONCAT(G22,F22),FALSE,A22:E22),G22)</f>
@@ -1030,23 +1051,23 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="D23" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="F23" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="G23" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="H23" t="str">
         <f>_xlfn.CONCAT(F23,_xlfn.TEXTJOIN(_xlfn.CONCAT(G23,F23),FALSE,A23:E23),G23)</f>
-        <v>&lt;c&gt;AES-KW&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;"cipher", "inverse"&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
+        <v>&lt;c&gt;AES-KW&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;["cipher", "inverse"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -1054,23 +1075,23 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="D24" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="F24" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="G24" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="H24" t="str">
         <f>_xlfn.CONCAT(F24,_xlfn.TEXTJOIN(_xlfn.CONCAT(G24,F24),FALSE,A24:E24),G24)</f>
-        <v>&lt;c&gt;AES-KWP&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;"cipher", "inverse"&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
+        <v>&lt;c&gt;AES-KWP&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;["cipher", "inverse"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -1078,23 +1099,23 @@
         <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="D25" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="E25" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F25" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="G25" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="H25" t="str">
         <f>_xlfn.CONCAT(F25,_xlfn.TEXTJOIN(_xlfn.CONCAT(G25,F25),FALSE,A25:E25),G25)</f>
-        <v>&lt;c&gt;TDES-KW&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;"cipher", "inverse"&lt;/c&gt;&lt;c&gt;1, 2 Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
+        <v>&lt;c&gt;TDES-KW&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;["cipher", "inverse"]&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -1129,10 +1150,10 @@
         <v>9</v>
       </c>
       <c r="K29" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="L29" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="M29" t="str">
         <f>_xlfn.CONCAT(K29,_xlfn.TEXTJOIN(_xlfn.CONCAT(L29,K29),FALSE,A29:J29),L29)</f>
@@ -1144,38 +1165,38 @@
         <v>22</v>
       </c>
       <c r="B30" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="C30" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="D30" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E30" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="F30" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="G30" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="I30" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="J30" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="K30" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="L30" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="M30" t="str">
         <f>_xlfn.CONCAT(K30,_xlfn.TEXTJOIN(_xlfn.CONCAT(L30,K30),FALSE,A30:J30),L30)</f>
-        <v>&lt;c&gt;AES-GCM&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;Min: 0, Max: 65536, Increment: any&lt;/c&gt;&lt;c&gt;Min: 8, Max: 1024, Increment: any&lt;/c&gt;&lt;c&gt;"internal", "external"&lt;/c&gt;&lt;c&gt;"8.2.1", "8.2.2"&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;Min: 0, Max: 65536, Increment: any&lt;/c&gt;&lt;c&gt;32, 64, 96, 104, 112, 120, 128&lt;/c&gt;</v>
+        <v>&lt;c&gt;AES-GCM&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;{"Min": 0, "Max": 65536, "Inc": any}&lt;/c&gt;&lt;c&gt;{"Min": 8, Max: 1024, Increment: any&lt;/c&gt;&lt;c&gt;["internal", "external"]&lt;/c&gt;&lt;c&gt;["8.2.1", "8.2.2"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;{"Min": 0, "Max": 65536, "Inc": any}&lt;/c&gt;&lt;c&gt;{[32, 64, 96, 104, 112, 120, 128]}&lt;/c&gt;</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -1183,74 +1204,74 @@
         <v>23</v>
       </c>
       <c r="B31" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="C31" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="D31" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="E31" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="F31" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="G31" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="H31" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="I31" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="J31" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="K31" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="L31" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="M31" t="str">
         <f>_xlfn.CONCAT(K31,_xlfn.TEXTJOIN(_xlfn.CONCAT(L31,K31),FALSE,A31:J31),L31)</f>
-        <v>&lt;c&gt;AES-XPN&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;Min: 1, Max: xxx, Increment: any&lt;/c&gt;&lt;c&gt;Min: 8, Max: 1024, Increment: any&lt;/c&gt;&lt;c&gt;"internal", "external"&lt;/c&gt;&lt;c&gt;"8.2.1", "8.2.2"&lt;/c&gt;&lt;c&gt;"internal", "external"&lt;/c&gt;&lt;c&gt;Min: 1, Max: any, Increment: any&lt;/c&gt;&lt;c&gt;32, 64, 96, 104, 112, 120, 128&lt;/c&gt;</v>
+        <v>&lt;c&gt;AES-XPN&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;{"Min": 1, "Max": xxx, "Inc": any}&lt;/c&gt;&lt;c&gt;{"Min": 8, "Max": 1024, "Inc": any}&lt;/c&gt;&lt;c&gt;["internal", "external"]&lt;/c&gt;&lt;c&gt;["8.2.1", "8.2.2"]&lt;/c&gt;&lt;c&gt;["internal", "external"]&lt;/c&gt;&lt;c&gt;{"Min": 1, "Max": any, "Inc": any}&lt;/c&gt;&lt;c&gt;{[32, 64, 96, 104, 112, 120, 128]}&lt;/c&gt;</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="C32" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="D32" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="E32" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="I32" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="J32" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="K32" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="L32" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="M32" t="str">
         <f>_xlfn.CONCAT(K32,_xlfn.TEXTJOIN(_xlfn.CONCAT(L32,K32),FALSE,A32:J32),L32)</f>
-        <v>&lt;c&gt;AES-CCM&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;Min: 0, Max: 256, Increment: 8&lt;/c&gt;&lt;c&gt;Min: 56, Max: 104, Increment: 8&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;Min: 0, Max: 524288, Increment: any&lt;/c&gt;&lt;c&gt;Min: 32, Max: 128, Increment: 16&lt;/c&gt;</v>
+        <v>&lt;c&gt;AES-CCM&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;{"Min": 0, "Max": 256, "Inc": 8}&lt;/c&gt;&lt;c&gt;{"Min": 56, "Max": 104, "Inc": 8}&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;{"Min": 0, "Max": 524288, "Inc": any}&lt;/c&gt;&lt;c&gt;{"Min": 32, "Max": 128, "Inc": 16}&lt;/c&gt;</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -1279,10 +1300,10 @@
         <v>14</v>
       </c>
       <c r="I36" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="J36" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="K36" t="str">
         <f>_xlfn.CONCAT(I36,_xlfn.TEXTJOIN(_xlfn.CONCAT(J36,I36),FALSE,A36:H36),J36)</f>
@@ -1294,56 +1315,56 @@
         <v>21</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="C37" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="D37" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="G37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I37" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="J37" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="K37" t="str">
         <f>_xlfn.CONCAT(I37,_xlfn.TEXTJOIN(_xlfn.CONCAT(J37,I37),FALSE,A37:H37),J37)</f>
-        <v>&lt;c&gt;AES-CTR&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;Min: 1, Max: 128, Increment: any&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;</v>
+        <v>&lt;c&gt;AES-CTR&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;{"Min": 1, "Max": 128, "Inc": any}&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="C38" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="D38" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E38" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="I38" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="J38" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="K38" t="str">
         <f>_xlfn.CONCAT(I38,_xlfn.TEXTJOIN(_xlfn.CONCAT(J38,I38),FALSE,A38:H38),J38)</f>
-        <v>&lt;c&gt;AES-XTS&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;128, 256&lt;/c&gt;&lt;c&gt;Min: 128, Max: 65536, Increment: 128&lt;/c&gt;&lt;c&gt;"hex", "number"&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
+        <v>&lt;c&gt;AES-XTS&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 256]&lt;/c&gt;&lt;c&gt;{"Min": 128, "Max": 65536, "Inc": 128}&lt;/c&gt;&lt;c&gt;["hex", "number"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -1351,29 +1372,29 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="D39" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="F39" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I39" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="J39" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="K39" t="str">
         <f>_xlfn.CONCAT(I39,_xlfn.TEXTJOIN(_xlfn.CONCAT(J39,I39),FALSE,A39:H39),J39)</f>
-        <v>&lt;c&gt;TDES-CTR&lt;/c&gt;&lt;c&gt;"encrypt", "decrypt"&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;Min: 1, Max: 64, Increment: any&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2 Note: 2 is only available for decrypt operations&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;</v>
+        <v>&lt;c&gt;TDES-CTR&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;{"Min": 1, "Max": 64, "Inc": any}&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;</v>
       </c>
     </row>
   </sheetData>
@@ -1386,7 +1407,7 @@
   <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1411,13 +1432,13 @@
         <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="E1" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="F1" t="str">
-        <f>_xlfn.CONCAT(D1,_xlfn.TEXTJOIN(_xlfn.CONCAT(E1,D1),FALSE,A1:C1),E1)</f>
+        <f t="shared" ref="F1:F18" si="0">_xlfn.CONCAT(D1,_xlfn.TEXTJOIN(_xlfn.CONCAT(E1,D1),FALSE,A1:C1),E1)</f>
         <v>&lt;ttcol align="left"&gt;algorithm&lt;/ttcol&gt;&lt;ttcol align="left"&gt;keyLen&lt;/ttcol&gt;&lt;ttcol align="left"&gt;keyingOption&lt;/ttcol&gt;</v>
       </c>
     </row>
@@ -1426,16 +1447,16 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E2" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F2" t="str">
-        <f>_xlfn.CONCAT(D2,_xlfn.TEXTJOIN(_xlfn.CONCAT(E2,D2),FALSE,A2:C2),E2)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;AES-ECB&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
       </c>
     </row>
@@ -1444,16 +1465,16 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F3" t="str">
-        <f>_xlfn.CONCAT(D3,_xlfn.TEXTJOIN(_xlfn.CONCAT(E3,D3),FALSE,A3:C3),E3)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;AES-CBC&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
       </c>
     </row>
@@ -1462,16 +1483,16 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F4" t="str">
-        <f>_xlfn.CONCAT(D4,_xlfn.TEXTJOIN(_xlfn.CONCAT(E4,D4),FALSE,A4:C4),E4)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;AES-OFB&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
       </c>
     </row>
@@ -1480,16 +1501,16 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F5" t="str">
-        <f>_xlfn.CONCAT(D5,_xlfn.TEXTJOIN(_xlfn.CONCAT(E5,D5),FALSE,A5:C5),E5)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;AES-CFB1&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
       </c>
     </row>
@@ -1498,16 +1519,16 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F6" t="str">
-        <f>_xlfn.CONCAT(D6,_xlfn.TEXTJOIN(_xlfn.CONCAT(E6,D6),FALSE,A6:C6),E6)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;AES-CFB8&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
       </c>
     </row>
@@ -1516,16 +1537,16 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E7" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F7" t="str">
-        <f>_xlfn.CONCAT(D7,_xlfn.TEXTJOIN(_xlfn.CONCAT(E7,D7),FALSE,A7:C7),E7)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;AES-CFB128&lt;/c&gt;&lt;c&gt;128, 192, 256&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
       </c>
     </row>
@@ -1534,16 +1555,16 @@
         <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F8" t="str">
-        <f>_xlfn.CONCAT(D8,_xlfn.TEXTJOIN(_xlfn.CONCAT(E8,D8),FALSE,A8:C8),E8)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;TDES-ECB&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2&lt;/c&gt;</v>
       </c>
     </row>
@@ -1552,16 +1573,16 @@
         <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E9" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F9" t="str">
-        <f>_xlfn.CONCAT(D9,_xlfn.TEXTJOIN(_xlfn.CONCAT(E9,D9),FALSE,A9:C9),E9)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;TDES-CBC&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2&lt;/c&gt;</v>
       </c>
     </row>
@@ -1570,16 +1591,16 @@
         <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F10" t="str">
-        <f>_xlfn.CONCAT(D10,_xlfn.TEXTJOIN(_xlfn.CONCAT(E10,D10),FALSE,A10:C10),E10)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;TDES-CBCI&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2&lt;/c&gt;</v>
       </c>
     </row>
@@ -1588,16 +1609,16 @@
         <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E11" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F11" t="str">
-        <f>_xlfn.CONCAT(D11,_xlfn.TEXTJOIN(_xlfn.CONCAT(E11,D11),FALSE,A11:C11),E11)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;TDES-CFB1&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2&lt;/c&gt;</v>
       </c>
     </row>
@@ -1606,16 +1627,16 @@
         <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="D12" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E12" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F12" t="str">
-        <f>_xlfn.CONCAT(D12,_xlfn.TEXTJOIN(_xlfn.CONCAT(E12,D12),FALSE,A12:C12),E12)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;TDES-CFB8&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2&lt;/c&gt;</v>
       </c>
     </row>
@@ -1624,16 +1645,16 @@
         <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E13" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F13" t="str">
-        <f>_xlfn.CONCAT(D13,_xlfn.TEXTJOIN(_xlfn.CONCAT(E13,D13),FALSE,A13:C13),E13)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;TDES-CFB64&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2&lt;/c&gt;</v>
       </c>
     </row>
@@ -1642,16 +1663,16 @@
         <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="D14" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E14" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F14" t="str">
-        <f>_xlfn.CONCAT(D14,_xlfn.TEXTJOIN(_xlfn.CONCAT(E14,D14),FALSE,A14:C14),E14)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;TDES-CFBP1&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2&lt;/c&gt;</v>
       </c>
     </row>
@@ -1660,16 +1681,16 @@
         <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="D15" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E15" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F15" t="str">
-        <f>_xlfn.CONCAT(D15,_xlfn.TEXTJOIN(_xlfn.CONCAT(E15,D15),FALSE,A15:C15),E15)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;TDES-CFBP8&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2&lt;/c&gt;</v>
       </c>
     </row>
@@ -1678,16 +1699,16 @@
         <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="D16" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E16" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F16" t="str">
-        <f>_xlfn.CONCAT(D16,_xlfn.TEXTJOIN(_xlfn.CONCAT(E16,D16),FALSE,A16:C16),E16)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;TDES-CFBP64&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2&lt;/c&gt;</v>
       </c>
     </row>
@@ -1696,16 +1717,16 @@
         <v>35</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E17" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F17" t="str">
-        <f>_xlfn.CONCAT(D17,_xlfn.TEXTJOIN(_xlfn.CONCAT(E17,D17),FALSE,A17:C17),E17)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;TDES-OFB&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2&lt;/c&gt;</v>
       </c>
     </row>
@@ -1714,16 +1735,16 @@
         <v>36</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E18" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F18" t="str">
-        <f>_xlfn.CONCAT(D18,_xlfn.TEXTJOIN(_xlfn.CONCAT(E18,D18),FALSE,A18:C18),E18)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;TDES-OFBI&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;1, 2&lt;/c&gt;</v>
       </c>
     </row>
@@ -1744,10 +1765,10 @@
         <v>3</v>
       </c>
       <c r="F22" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="G22" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="H22" t="str">
         <f>_xlfn.CONCAT(F22,_xlfn.TEXTJOIN(_xlfn.CONCAT(G22,F22),FALSE,A22:E22),G22)</f>
@@ -1759,19 +1780,19 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D23" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E23" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="F23" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="G23" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="H23" t="str">
         <f>_xlfn.CONCAT(F23,_xlfn.TEXTJOIN(_xlfn.CONCAT(G23,F23),FALSE,A23:E23),G23)</f>
@@ -1783,19 +1804,19 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D24" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E24" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="F24" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="G24" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="H24" t="str">
         <f>_xlfn.CONCAT(F24,_xlfn.TEXTJOIN(_xlfn.CONCAT(G24,F24),FALSE,A24:E24),G24)</f>
@@ -1807,19 +1828,19 @@
         <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="D25" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E25" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="F25" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="G25" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="H25" t="str">
         <f>_xlfn.CONCAT(F25,_xlfn.TEXTJOIN(_xlfn.CONCAT(G25,F25),FALSE,A25:E25),G25)</f>
@@ -1855,13 +1876,13 @@
         <v>9</v>
       </c>
       <c r="J29" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="K29" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="L29" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="M29" t="str">
         <f>_xlfn.CONCAT(K29,_xlfn.TEXTJOIN(_xlfn.CONCAT(L29,K29),FALSE,A29:J29),L29)</f>
@@ -1873,31 +1894,31 @@
         <v>22</v>
       </c>
       <c r="B30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C30" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" t="s">
         <v>45</v>
       </c>
-      <c r="D30" t="s">
-        <v>46</v>
-      </c>
       <c r="F30" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="G30" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="H30" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="I30" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="K30" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="L30" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="M30" t="str">
         <f>_xlfn.CONCAT(K30,_xlfn.TEXTJOIN(_xlfn.CONCAT(L30,K30),FALSE,A30:J30),L30)</f>
@@ -1909,37 +1930,37 @@
         <v>23</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" t="s">
         <v>45</v>
       </c>
-      <c r="D31" t="s">
-        <v>46</v>
-      </c>
       <c r="E31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F31" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="G31" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="H31" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="I31" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="J31" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="K31" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="L31" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="M31" t="str">
         <f>_xlfn.CONCAT(K31,_xlfn.TEXTJOIN(_xlfn.CONCAT(L31,K31),FALSE,A31:J31),L31)</f>
@@ -1948,28 +1969,28 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F32" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="G32" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="H32" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="I32" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="K32" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="L32" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="M32" t="str">
         <f>_xlfn.CONCAT(K32,_xlfn.TEXTJOIN(_xlfn.CONCAT(L32,K32),FALSE,A32:J32),L32)</f>
@@ -1987,10 +2008,10 @@
         <v>12</v>
       </c>
       <c r="D36" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="E36" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="F36" t="s">
         <v>11</v>
@@ -1999,10 +2020,10 @@
         <v>3</v>
       </c>
       <c r="H36" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="I36" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="J36" t="str">
         <f>_xlfn.CONCAT(H36,_xlfn.TEXTJOIN(_xlfn.CONCAT(I36,H36),FALSE,A36:G36),I36)</f>
@@ -2014,19 +2035,19 @@
         <v>21</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H37" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="I37" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="J37" t="str">
         <f>_xlfn.CONCAT(H37,_xlfn.TEXTJOIN(_xlfn.CONCAT(I37,H37),FALSE,A37:G37),I37)</f>
@@ -2035,22 +2056,22 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" t="s">
+        <v>40</v>
+      </c>
+      <c r="F38" t="s">
         <v>43</v>
       </c>
-      <c r="B38" t="s">
-        <v>41</v>
-      </c>
-      <c r="F38" t="s">
-        <v>44</v>
-      </c>
       <c r="G38" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="H38" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="I38" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="J38" t="str">
         <f>_xlfn.CONCAT(H38,_xlfn.TEXTJOIN(_xlfn.CONCAT(I38,H38),FALSE,A38:G38),I38)</f>
@@ -2062,19 +2083,19 @@
         <v>37</v>
       </c>
       <c r="C39" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="D39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H39" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="I39" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="J39" t="str">
         <f>_xlfn.CONCAT(H39,_xlfn.TEXTJOIN(_xlfn.CONCAT(I39,H39),FALSE,A39:G39),I39)</f>

</xml_diff>

<commit_message>
Updates property tables and examples
</commit_message>
<xml_diff>
--- a/tools/SpecBook.xlsx
+++ b/tools/SpecBook.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentation-ACVP\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{94F91522-14C5-4208-8440-478E1BEC7FAB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BAA27522-B8C1-4BE1-926B-686466604EF1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7050" activeTab="1" xr2:uid="{4A423B63-A7B8-4728-A188-1056F06A2A15}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7050" activeTab="2" xr2:uid="{4A423B63-A7B8-4728-A188-1056F06A2A15}"/>
   </bookViews>
   <sheets>
     <sheet name="Symmetric Registration" sheetId="1" r:id="rId1"/>
     <sheet name="Symmetric Prompt Test Group" sheetId="2" r:id="rId2"/>
+    <sheet name="SHA3-SHAKE Registration" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="89">
   <si>
     <t>algorithm</t>
   </si>
@@ -260,6 +261,39 @@
   </si>
   <si>
     <t>{"Min": 32, "Max": 128, "Inc": 16}</t>
+  </si>
+  <si>
+    <t>inBit</t>
+  </si>
+  <si>
+    <t>inEmpty</t>
+  </si>
+  <si>
+    <t>outLength</t>
+  </si>
+  <si>
+    <t>outBit</t>
+  </si>
+  <si>
+    <t>SHA3-224</t>
+  </si>
+  <si>
+    <t>SHA3-256</t>
+  </si>
+  <si>
+    <t>SHA3-384</t>
+  </si>
+  <si>
+    <t>SHA3-512</t>
+  </si>
+  <si>
+    <t>SHAKE-128</t>
+  </si>
+  <si>
+    <t>SHAKE-256</t>
+  </si>
+  <si>
+    <t>{"Min": 16, "Max": 65536, "Inc": any}</t>
   </si>
 </sst>
 </file>
@@ -614,7 +648,7 @@
   <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29:M32"/>
+      <selection activeCell="E1" sqref="E1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1406,7 +1440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4BEB1AA-8A6E-4317-A406-8B0373CC58E9}">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -2105,4 +2139,191 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6147422C-C6BB-4B90-9E5E-89D3819A0EF0}">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" t="str">
+        <f>_xlfn.CONCAT(F1,_xlfn.TEXTJOIN(_xlfn.CONCAT(G1,F1),,A1:E1),G1)</f>
+        <v>&lt;ttcol align="left"&gt;algorithm&lt;/ttcol&gt;&lt;ttcol align="left"&gt;inBit&lt;/ttcol&gt;&lt;ttcol align="left"&gt;inEmpty&lt;/ttcol&gt;&lt;ttcol align="left"&gt;outLength&lt;/ttcol&gt;&lt;ttcol align="left"&gt;outBit&lt;/ttcol&gt;</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" t="str">
+        <f>_xlfn.CONCAT(F2,_xlfn.TEXTJOIN(_xlfn.CONCAT(G2,F2),FALSE,A2:E2),G2)</f>
+        <v>&lt;c&gt;SHA3-224&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" t="str">
+        <f>_xlfn.CONCAT(F3,_xlfn.TEXTJOIN(_xlfn.CONCAT(G3,F3),FALSE,A3:E3),G3)</f>
+        <v>&lt;c&gt;SHA3-256&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" t="str">
+        <f>_xlfn.CONCAT(F4,_xlfn.TEXTJOIN(_xlfn.CONCAT(G4,F4),FALSE,A4:E4),G4)</f>
+        <v>&lt;c&gt;SHA3-384&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" t="str">
+        <f>_xlfn.CONCAT(F5,_xlfn.TEXTJOIN(_xlfn.CONCAT(G5,F5),FALSE,A5:E5),G5)</f>
+        <v>&lt;c&gt;SHA3-512&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" t="str">
+        <f>_xlfn.CONCAT(F6,_xlfn.TEXTJOIN(_xlfn.CONCAT(G6,F6),FALSE,A6:E6),G6)</f>
+        <v>&lt;c&gt;SHAKE-128&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;{"Min": 16, "Max": 65536, "Inc": any}&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" t="str">
+        <f>_xlfn.CONCAT(F7,_xlfn.TEXTJOIN(_xlfn.CONCAT(G7,F7),FALSE,A7:E7),G7)</f>
+        <v>&lt;c&gt;SHAKE-256&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;{"Min": 16, "Max": 65536, "Inc": any}&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updates Excel sheet with tables for Symmetric spec
</commit_message>
<xml_diff>
--- a/tools/SpecBook.xlsx
+++ b/tools/SpecBook.xlsx
@@ -1,33 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentation-ACVP\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BAA27522-B8C1-4BE1-926B-686466604EF1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83B2B68-113A-4D59-AA38-CE5A5C65AC4E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7050" activeTab="2" xr2:uid="{4A423B63-A7B8-4728-A188-1056F06A2A15}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7050" xr2:uid="{4A423B63-A7B8-4728-A188-1056F06A2A15}"/>
   </bookViews>
   <sheets>
     <sheet name="Symmetric Registration" sheetId="1" r:id="rId1"/>
     <sheet name="Symmetric Prompt Test Group" sheetId="2" r:id="rId2"/>
     <sheet name="SHA3-SHAKE Registration" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="91">
   <si>
     <t>algorithm</t>
   </si>
@@ -218,9 +223,6 @@
     <t>{"Min": 0, "Max": 65536, "Inc": any}</t>
   </si>
   <si>
-    <t>{"Min": 1, "Max": xxx, "Inc": any}</t>
-  </si>
-  <si>
     <t>{"Min": 0, "Max": 256, "Inc": 8}</t>
   </si>
   <si>
@@ -294,6 +296,15 @@
   </si>
   <si>
     <t>{"Min": 16, "Max": 65536, "Inc": any}</t>
+  </si>
+  <si>
+    <t>revision</t>
+  </si>
+  <si>
+    <t>"1.0.0"</t>
+  </si>
+  <si>
+    <t>{"Min": 1, "Max": 65536, "Inc": any}</t>
   </si>
 </sst>
 </file>
@@ -645,790 +656,881 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACB07B3C-5951-470E-AC11-4876B2F0E9E2}">
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:G2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N29" sqref="N29:N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="48.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>48</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>49</v>
       </c>
-      <c r="G1" t="str">
-        <f>_xlfn.CONCAT(E1,_xlfn.TEXTJOIN(_xlfn.CONCAT(F1,E1),,A1:D1),F1)</f>
-        <v>&lt;ttcol align="left"&gt;algorithm&lt;/ttcol&gt;&lt;ttcol align="left"&gt;direction&lt;/ttcol&gt;&lt;ttcol align="left"&gt;keyLen&lt;/ttcol&gt;&lt;ttcol align="left"&gt;keyingOption&lt;/ttcol&gt;</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="str">
+        <f>_xlfn.CONCAT(F1,_xlfn.TEXTJOIN(_xlfn.CONCAT(G1,F1),,A1:E1),G1)</f>
+        <v>&lt;ttcol align="left"&gt;algorithm&lt;/ttcol&gt;&lt;ttcol align="left"&gt;revision&lt;/ttcol&gt;&lt;ttcol align="left"&gt;direction&lt;/ttcol&gt;&lt;ttcol align="left"&gt;keyLen&lt;/ttcol&gt;&lt;ttcol align="left"&gt;keyingOption&lt;/ttcol&gt;</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" t="s">
         <v>57</v>
       </c>
-      <c r="E2" t="s">
-        <v>50</v>
-      </c>
       <c r="F2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G2" t="str">
-        <f t="shared" ref="G2:G18" si="0">_xlfn.CONCAT(E2,_xlfn.TEXTJOIN(_xlfn.CONCAT(F2,E2),FALSE,A2:D2),F2)</f>
-        <v>&lt;c&gt;AES-ECB&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="G2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" t="str">
+        <f t="shared" ref="H2:H18" si="0">_xlfn.CONCAT(F2,_xlfn.TEXTJOIN(_xlfn.CONCAT(G2,F2),FALSE,A2:E2),G2)</f>
+        <v>&lt;c&gt;AES-ECB&lt;/c&gt;&lt;c&gt;"1.0.0"&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
         <v>57</v>
       </c>
-      <c r="E3" t="s">
-        <v>50</v>
-      </c>
       <c r="F3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;c&gt;AES-CBC&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="G3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;c&gt;AES-CBC&lt;/c&gt;&lt;c&gt;"1.0.0"&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="C4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" t="s">
         <v>57</v>
       </c>
-      <c r="E4" t="s">
-        <v>50</v>
-      </c>
       <c r="F4" t="s">
-        <v>51</v>
-      </c>
-      <c r="G4" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;c&gt;AES-OFB&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="G4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;c&gt;AES-OFB&lt;/c&gt;&lt;c&gt;"1.0.0"&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" t="s">
         <v>57</v>
       </c>
-      <c r="E5" t="s">
-        <v>50</v>
-      </c>
       <c r="F5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G5" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;c&gt;AES-CFB1&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="G5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;c&gt;AES-CFB1&lt;/c&gt;&lt;c&gt;"1.0.0"&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" t="s">
         <v>57</v>
       </c>
-      <c r="E6" t="s">
-        <v>50</v>
-      </c>
       <c r="F6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G6" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;c&gt;AES-CFB8&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="G6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;c&gt;AES-CFB8&lt;/c&gt;&lt;c&gt;"1.0.0"&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="C7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" t="s">
         <v>57</v>
       </c>
-      <c r="E7" t="s">
-        <v>50</v>
-      </c>
       <c r="F7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;c&gt;AES-CFB128&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="G7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;c&gt;AES-CFB128&lt;/c&gt;&lt;c&gt;"1.0.0"&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" t="s">
         <v>59</v>
       </c>
-      <c r="E8" t="s">
-        <v>50</v>
-      </c>
       <c r="F8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G8" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;c&gt;TDES-ECB&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="G8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;c&gt;TDES-ECB&lt;/c&gt;&lt;c&gt;"1.0.0"&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" t="s">
         <v>59</v>
       </c>
-      <c r="E9" t="s">
-        <v>50</v>
-      </c>
       <c r="F9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G9" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;c&gt;TDES-CBC&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="G9" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;c&gt;TDES-CBC&lt;/c&gt;&lt;c&gt;"1.0.0"&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" t="s">
         <v>59</v>
       </c>
-      <c r="E10" t="s">
-        <v>50</v>
-      </c>
       <c r="F10" t="s">
-        <v>51</v>
-      </c>
-      <c r="G10" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;c&gt;TDES-CBCI&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="G10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;c&gt;TDES-CBCI&lt;/c&gt;&lt;c&gt;"1.0.0"&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" t="s">
         <v>59</v>
       </c>
-      <c r="E11" t="s">
-        <v>50</v>
-      </c>
       <c r="F11" t="s">
-        <v>51</v>
-      </c>
-      <c r="G11" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;c&gt;TDES-CFB1&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="G11" t="s">
+        <v>51</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;c&gt;TDES-CFB1&lt;/c&gt;&lt;c&gt;"1.0.0"&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" t="s">
         <v>59</v>
       </c>
-      <c r="E12" t="s">
-        <v>50</v>
-      </c>
       <c r="F12" t="s">
-        <v>51</v>
-      </c>
-      <c r="G12" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;c&gt;TDES-CFB8&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="G12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;c&gt;TDES-CFB8&lt;/c&gt;&lt;c&gt;"1.0.0"&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" t="s">
         <v>59</v>
       </c>
-      <c r="E13" t="s">
-        <v>50</v>
-      </c>
       <c r="F13" t="s">
-        <v>51</v>
-      </c>
-      <c r="G13" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;c&gt;TDES-CFB64&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="G13" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;c&gt;TDES-CFB64&lt;/c&gt;&lt;c&gt;"1.0.0"&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" t="s">
         <v>59</v>
       </c>
-      <c r="E14" t="s">
-        <v>50</v>
-      </c>
       <c r="F14" t="s">
-        <v>51</v>
-      </c>
-      <c r="G14" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;c&gt;TDES-CFBP1&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="G14" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;c&gt;TDES-CFBP1&lt;/c&gt;&lt;c&gt;"1.0.0"&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" t="s">
         <v>59</v>
       </c>
-      <c r="E15" t="s">
-        <v>50</v>
-      </c>
       <c r="F15" t="s">
-        <v>51</v>
-      </c>
-      <c r="G15" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;c&gt;TDES-CFBP8&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="G15" t="s">
+        <v>51</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;c&gt;TDES-CFBP8&lt;/c&gt;&lt;c&gt;"1.0.0"&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" t="s">
         <v>59</v>
       </c>
-      <c r="E16" t="s">
-        <v>50</v>
-      </c>
       <c r="F16" t="s">
-        <v>51</v>
-      </c>
-      <c r="G16" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;c&gt;TDES-CFBP64&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="G16" t="s">
+        <v>51</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;c&gt;TDES-CFBP64&lt;/c&gt;&lt;c&gt;"1.0.0"&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" t="s">
         <v>59</v>
       </c>
-      <c r="E17" t="s">
-        <v>50</v>
-      </c>
       <c r="F17" t="s">
-        <v>51</v>
-      </c>
-      <c r="G17" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;c&gt;TDES-OFB&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="G17" t="s">
+        <v>51</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;c&gt;TDES-OFB&lt;/c&gt;&lt;c&gt;"1.0.0"&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" t="s">
         <v>59</v>
       </c>
-      <c r="E18" t="s">
-        <v>50</v>
-      </c>
       <c r="F18" t="s">
-        <v>51</v>
-      </c>
-      <c r="G18" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;c&gt;TDES-OFBI&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="G18" t="s">
+        <v>51</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;c&gt;TDES-OFBI&lt;/c&gt;&lt;c&gt;"1.0.0"&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
       <c r="B22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" t="s">
         <v>1</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>2</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>10</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>12</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>48</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>49</v>
       </c>
-      <c r="H22" t="str">
-        <f>_xlfn.CONCAT(F22,_xlfn.TEXTJOIN(_xlfn.CONCAT(G22,F22),FALSE,A22:E22),G22)</f>
-        <v>&lt;ttcol align="left"&gt;algorithm&lt;/ttcol&gt;&lt;ttcol align="left"&gt;direction&lt;/ttcol&gt;&lt;ttcol align="left"&gt;keyLen&lt;/ttcol&gt;&lt;ttcol align="left"&gt;kwCipher&lt;/ttcol&gt;&lt;ttcol align="left"&gt;keyingOption&lt;/ttcol&gt;</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I22" t="str">
+        <f>_xlfn.CONCAT(G22,_xlfn.TEXTJOIN(_xlfn.CONCAT(H22,G22),FALSE,A22:F22),H22)</f>
+        <v>&lt;ttcol align="left"&gt;algorithm&lt;/ttcol&gt;&lt;ttcol align="left"&gt;revision&lt;/ttcol&gt;&lt;ttcol align="left"&gt;direction&lt;/ttcol&gt;&lt;ttcol align="left"&gt;keyLen&lt;/ttcol&gt;&lt;ttcol align="left"&gt;kwCipher&lt;/ttcol&gt;&lt;ttcol align="left"&gt;keyingOption&lt;/ttcol&gt;</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="C23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" t="s">
         <v>57</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>61</v>
       </c>
-      <c r="F23" t="s">
-        <v>50</v>
-      </c>
       <c r="G23" t="s">
-        <v>51</v>
-      </c>
-      <c r="H23" t="str">
-        <f>_xlfn.CONCAT(F23,_xlfn.TEXTJOIN(_xlfn.CONCAT(G23,F23),FALSE,A23:E23),G23)</f>
-        <v>&lt;c&gt;AES-KW&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;["cipher", "inverse"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="H23" t="s">
+        <v>51</v>
+      </c>
+      <c r="I23" t="str">
+        <f>_xlfn.CONCAT(G23,_xlfn.TEXTJOIN(_xlfn.CONCAT(H23,G23),FALSE,A23:F23),H23)</f>
+        <v>&lt;c&gt;AES-KW&lt;/c&gt;&lt;c&gt;"1.0.0"&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;["cipher", "inverse"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="C24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" t="s">
         <v>57</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>61</v>
       </c>
-      <c r="F24" t="s">
-        <v>50</v>
-      </c>
       <c r="G24" t="s">
-        <v>51</v>
-      </c>
-      <c r="H24" t="str">
-        <f>_xlfn.CONCAT(F24,_xlfn.TEXTJOIN(_xlfn.CONCAT(G24,F24),FALSE,A24:E24),G24)</f>
-        <v>&lt;c&gt;AES-KWP&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;["cipher", "inverse"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="H24" t="s">
+        <v>51</v>
+      </c>
+      <c r="I24" t="str">
+        <f>_xlfn.CONCAT(G24,_xlfn.TEXTJOIN(_xlfn.CONCAT(H24,G24),FALSE,A24:F24),H24)</f>
+        <v>&lt;c&gt;AES-KWP&lt;/c&gt;&lt;c&gt;"1.0.0"&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;["cipher", "inverse"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>58</v>
-      </c>
-      <c r="D25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" t="s">
         <v>61</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>59</v>
       </c>
-      <c r="F25" t="s">
-        <v>50</v>
-      </c>
       <c r="G25" t="s">
-        <v>51</v>
-      </c>
-      <c r="H25" t="str">
-        <f>_xlfn.CONCAT(F25,_xlfn.TEXTJOIN(_xlfn.CONCAT(G25,F25),FALSE,A25:E25),G25)</f>
-        <v>&lt;c&gt;TDES-KW&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;["cipher", "inverse"]&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="H25" t="s">
+        <v>51</v>
+      </c>
+      <c r="I25" t="str">
+        <f>_xlfn.CONCAT(G25,_xlfn.TEXTJOIN(_xlfn.CONCAT(H25,G25),FALSE,A25:F25),H25)</f>
+        <v>&lt;c&gt;TDES-KW&lt;/c&gt;&lt;c&gt;"1.0.0"&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;["cipher", "inverse"]&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>0</v>
       </c>
       <c r="B29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" t="s">
         <v>1</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>2</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>3</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>4</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>5</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>6</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>7</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
         <v>8</v>
       </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
         <v>9</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
         <v>48</v>
       </c>
-      <c r="L29" t="s">
+      <c r="M29" t="s">
         <v>49</v>
       </c>
-      <c r="M29" t="str">
-        <f>_xlfn.CONCAT(K29,_xlfn.TEXTJOIN(_xlfn.CONCAT(L29,K29),FALSE,A29:J29),L29)</f>
-        <v>&lt;ttcol align="left"&gt;algorithm&lt;/ttcol&gt;&lt;ttcol align="left"&gt;direction&lt;/ttcol&gt;&lt;ttcol align="left"&gt;keyLen&lt;/ttcol&gt;&lt;ttcol align="left"&gt;dataLen&lt;/ttcol&gt;&lt;ttcol align="left"&gt;ivLen&lt;/ttcol&gt;&lt;ttcol align="left"&gt;ivGen&lt;/ttcol&gt;&lt;ttcol align="left"&gt;ivGenMode&lt;/ttcol&gt;&lt;ttcol align="left"&gt;saltGen&lt;/ttcol&gt;&lt;ttcol align="left"&gt;aadLen&lt;/ttcol&gt;&lt;ttcol align="left"&gt;tagLen&lt;/ttcol&gt;</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N29" t="str">
+        <f>_xlfn.CONCAT(L29,_xlfn.TEXTJOIN(_xlfn.CONCAT(M29,L29),FALSE,A29:K29),M29)</f>
+        <v>&lt;ttcol align="left"&gt;algorithm&lt;/ttcol&gt;&lt;ttcol align="left"&gt;revision&lt;/ttcol&gt;&lt;ttcol align="left"&gt;direction&lt;/ttcol&gt;&lt;ttcol align="left"&gt;keyLen&lt;/ttcol&gt;&lt;ttcol align="left"&gt;dataLen&lt;/ttcol&gt;&lt;ttcol align="left"&gt;ivLen&lt;/ttcol&gt;&lt;ttcol align="left"&gt;ivGen&lt;/ttcol&gt;&lt;ttcol align="left"&gt;ivGenMode&lt;/ttcol&gt;&lt;ttcol align="left"&gt;saltGen&lt;/ttcol&gt;&lt;ttcol align="left"&gt;aadLen&lt;/ttcol&gt;&lt;ttcol align="left"&gt;tagLen&lt;/ttcol&gt;</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>22</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="C30" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" t="s">
         <v>57</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>62</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
+        <v>68</v>
+      </c>
+      <c r="G30" t="s">
         <v>69</v>
       </c>
-      <c r="F30" t="s">
+      <c r="H30" t="s">
         <v>70</v>
       </c>
-      <c r="G30" t="s">
+      <c r="J30" t="s">
+        <v>62</v>
+      </c>
+      <c r="K30" t="s">
         <v>71</v>
       </c>
-      <c r="I30" t="s">
-        <v>62</v>
-      </c>
-      <c r="J30" t="s">
-        <v>72</v>
-      </c>
-      <c r="K30" t="s">
-        <v>50</v>
-      </c>
       <c r="L30" t="s">
-        <v>51</v>
-      </c>
-      <c r="M30" t="str">
-        <f>_xlfn.CONCAT(K30,_xlfn.TEXTJOIN(_xlfn.CONCAT(L30,K30),FALSE,A30:J30),L30)</f>
-        <v>&lt;c&gt;AES-GCM&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;{"Min": 0, "Max": 65536, "Inc": any}&lt;/c&gt;&lt;c&gt;{"Min": 8, Max: 1024, Increment: any&lt;/c&gt;&lt;c&gt;["internal", "external"]&lt;/c&gt;&lt;c&gt;["8.2.1", "8.2.2"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;{"Min": 0, "Max": 65536, "Inc": any}&lt;/c&gt;&lt;c&gt;{[32, 64, 96, 104, 112, 120, 128]}&lt;/c&gt;</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="M30" t="s">
+        <v>51</v>
+      </c>
+      <c r="N30" t="str">
+        <f>_xlfn.CONCAT(L30,_xlfn.TEXTJOIN(_xlfn.CONCAT(M30,L30),FALSE,A30:K30),M30)</f>
+        <v>&lt;c&gt;AES-GCM&lt;/c&gt;&lt;c&gt;"1.0.0"&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;{"Min": 0, "Max": 65536, "Inc": any}&lt;/c&gt;&lt;c&gt;{"Min": 8, Max: 1024, Increment: any&lt;/c&gt;&lt;c&gt;["internal", "external"]&lt;/c&gt;&lt;c&gt;["8.2.1", "8.2.2"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;{"Min": 0, "Max": 65536, "Inc": any}&lt;/c&gt;&lt;c&gt;{[32, 64, 96, 104, 112, 120, 128]}&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>23</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="C31" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" t="s">
         <v>57</v>
       </c>
-      <c r="D31" t="s">
-        <v>63</v>
-      </c>
       <c r="E31" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="F31" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G31" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H31" t="s">
         <v>70</v>
       </c>
       <c r="I31" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="J31" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="K31" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="L31" t="s">
-        <v>51</v>
-      </c>
-      <c r="M31" t="str">
-        <f>_xlfn.CONCAT(K31,_xlfn.TEXTJOIN(_xlfn.CONCAT(L31,K31),FALSE,A31:J31),L31)</f>
-        <v>&lt;c&gt;AES-XPN&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;{"Min": 1, "Max": xxx, "Inc": any}&lt;/c&gt;&lt;c&gt;{"Min": 8, "Max": 1024, "Inc": any}&lt;/c&gt;&lt;c&gt;["internal", "external"]&lt;/c&gt;&lt;c&gt;["8.2.1", "8.2.2"]&lt;/c&gt;&lt;c&gt;["internal", "external"]&lt;/c&gt;&lt;c&gt;{"Min": 1, "Max": any, "Inc": any}&lt;/c&gt;&lt;c&gt;{[32, 64, 96, 104, 112, 120, 128]}&lt;/c&gt;</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="M31" t="s">
+        <v>51</v>
+      </c>
+      <c r="N31" t="str">
+        <f>_xlfn.CONCAT(L31,_xlfn.TEXTJOIN(_xlfn.CONCAT(M31,L31),FALSE,A31:K31),M31)</f>
+        <v>&lt;c&gt;AES-XPN&lt;/c&gt;&lt;c&gt;"1.0.0"&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;{"Min": 1, "Max": 65536, "Inc": any}&lt;/c&gt;&lt;c&gt;{"Min": 8, "Max": 1024, "Inc": any}&lt;/c&gt;&lt;c&gt;["internal", "external"]&lt;/c&gt;&lt;c&gt;["8.2.1", "8.2.2"]&lt;/c&gt;&lt;c&gt;["internal", "external"]&lt;/c&gt;&lt;c&gt;{"Min": 1, "Max": any, "Inc": any}&lt;/c&gt;&lt;c&gt;{[32, 64, 96, 104, 112, 120, 128]}&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>46</v>
       </c>
       <c r="B32" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="C32" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" t="s">
         <v>57</v>
       </c>
-      <c r="D32" t="s">
-        <v>64</v>
-      </c>
       <c r="E32" t="s">
-        <v>74</v>
-      </c>
-      <c r="I32" t="s">
+        <v>63</v>
+      </c>
+      <c r="F32" t="s">
+        <v>73</v>
+      </c>
+      <c r="J32" t="s">
+        <v>75</v>
+      </c>
+      <c r="K32" t="s">
         <v>76</v>
       </c>
-      <c r="J32" t="s">
-        <v>77</v>
-      </c>
-      <c r="K32" t="s">
-        <v>50</v>
-      </c>
       <c r="L32" t="s">
-        <v>51</v>
-      </c>
-      <c r="M32" t="str">
-        <f>_xlfn.CONCAT(K32,_xlfn.TEXTJOIN(_xlfn.CONCAT(L32,K32),FALSE,A32:J32),L32)</f>
-        <v>&lt;c&gt;AES-CCM&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;{"Min": 0, "Max": 256, "Inc": 8}&lt;/c&gt;&lt;c&gt;{"Min": 56, "Max": 104, "Inc": 8}&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;{"Min": 0, "Max": 524288, "Inc": any}&lt;/c&gt;&lt;c&gt;{"Min": 32, "Max": 128, "Inc": 16}&lt;/c&gt;</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="M32" t="s">
+        <v>51</v>
+      </c>
+      <c r="N32" t="str">
+        <f>_xlfn.CONCAT(L32,_xlfn.TEXTJOIN(_xlfn.CONCAT(M32,L32),FALSE,A32:K32),M32)</f>
+        <v>&lt;c&gt;AES-CCM&lt;/c&gt;&lt;c&gt;"1.0.0"&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;{"Min": 0, "Max": 256, "Inc": 8}&lt;/c&gt;&lt;c&gt;{"Min": 56, "Max": 104, "Inc": 8}&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;{"Min": 0, "Max": 524288, "Inc": any}&lt;/c&gt;&lt;c&gt;{"Min": 32, "Max": 128, "Inc": 16}&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>0</v>
       </c>
       <c r="B36" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36" t="s">
         <v>1</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>2</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>3</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>11</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>12</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>13</v>
       </c>
-      <c r="H36" t="s">
+      <c r="I36" t="s">
         <v>14</v>
       </c>
-      <c r="I36" t="s">
+      <c r="J36" t="s">
         <v>48</v>
       </c>
-      <c r="J36" t="s">
+      <c r="K36" t="s">
         <v>49</v>
       </c>
-      <c r="K36" t="str">
-        <f>_xlfn.CONCAT(I36,_xlfn.TEXTJOIN(_xlfn.CONCAT(J36,I36),FALSE,A36:H36),J36)</f>
-        <v>&lt;ttcol align="left"&gt;algorithm&lt;/ttcol&gt;&lt;ttcol align="left"&gt;direction&lt;/ttcol&gt;&lt;ttcol align="left"&gt;keyLen&lt;/ttcol&gt;&lt;ttcol align="left"&gt;dataLen&lt;/ttcol&gt;&lt;ttcol align="left"&gt;tweakMode&lt;/ttcol&gt;&lt;ttcol align="left"&gt;keyingOption&lt;/ttcol&gt;&lt;ttcol align="left"&gt;overflowCounter&lt;/ttcol&gt;&lt;ttcol align="left"&gt;incrementalCounter&lt;/ttcol&gt;</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L36" t="str">
+        <f>_xlfn.CONCAT(J36,_xlfn.TEXTJOIN(_xlfn.CONCAT(K36,J36),FALSE,A36:I36),K36)</f>
+        <v>&lt;ttcol align="left"&gt;algorithm&lt;/ttcol&gt;&lt;ttcol align="left"&gt;revision&lt;/ttcol&gt;&lt;ttcol align="left"&gt;direction&lt;/ttcol&gt;&lt;ttcol align="left"&gt;keyLen&lt;/ttcol&gt;&lt;ttcol align="left"&gt;dataLen&lt;/ttcol&gt;&lt;ttcol align="left"&gt;tweakMode&lt;/ttcol&gt;&lt;ttcol align="left"&gt;keyingOption&lt;/ttcol&gt;&lt;ttcol align="left"&gt;overflowCounter&lt;/ttcol&gt;&lt;ttcol align="left"&gt;incrementalCounter&lt;/ttcol&gt;</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>21</v>
       </c>
       <c r="B37" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="C37" t="s">
+        <v>58</v>
+      </c>
+      <c r="D37" t="s">
         <v>57</v>
       </c>
-      <c r="D37" t="s">
-        <v>68</v>
-      </c>
-      <c r="G37" t="s">
-        <v>41</v>
+      <c r="E37" t="s">
+        <v>67</v>
       </c>
       <c r="H37" t="s">
         <v>41</v>
       </c>
       <c r="I37" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="J37" t="s">
-        <v>51</v>
-      </c>
-      <c r="K37" t="str">
-        <f>_xlfn.CONCAT(I37,_xlfn.TEXTJOIN(_xlfn.CONCAT(J37,I37),FALSE,A37:H37),J37)</f>
-        <v>&lt;c&gt;AES-CTR&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;{"Min": 1, "Max": 128, "Inc": any}&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="K37" t="s">
+        <v>51</v>
+      </c>
+      <c r="L37" t="str">
+        <f>_xlfn.CONCAT(J37,_xlfn.TEXTJOIN(_xlfn.CONCAT(K37,J37),FALSE,A37:I37),K37)</f>
+        <v>&lt;c&gt;AES-CTR&lt;/c&gt;&lt;c&gt;"1.0.0"&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 192, 256]&lt;/c&gt;&lt;c&gt;{"Min": 1, "Max": 128, "Inc": any}&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>42</v>
       </c>
       <c r="B38" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="C38" t="s">
+        <v>58</v>
+      </c>
+      <c r="D38" t="s">
         <v>60</v>
       </c>
-      <c r="D38" t="s">
-        <v>65</v>
-      </c>
       <c r="E38" t="s">
-        <v>67</v>
-      </c>
-      <c r="I38" t="s">
-        <v>50</v>
+        <v>64</v>
+      </c>
+      <c r="F38" t="s">
+        <v>66</v>
       </c>
       <c r="J38" t="s">
-        <v>51</v>
-      </c>
-      <c r="K38" t="str">
-        <f>_xlfn.CONCAT(I38,_xlfn.TEXTJOIN(_xlfn.CONCAT(J38,I38),FALSE,A38:H38),J38)</f>
-        <v>&lt;c&gt;AES-XTS&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 256]&lt;/c&gt;&lt;c&gt;{"Min": 128, "Max": 65536, "Inc": 128}&lt;/c&gt;&lt;c&gt;["hex", "number"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="K38" t="s">
+        <v>51</v>
+      </c>
+      <c r="L38" t="str">
+        <f>_xlfn.CONCAT(J38,_xlfn.TEXTJOIN(_xlfn.CONCAT(K38,J38),FALSE,A38:I38),K38)</f>
+        <v>&lt;c&gt;AES-XTS&lt;/c&gt;&lt;c&gt;"1.0.0"&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;[128, 256]&lt;/c&gt;&lt;c&gt;{"Min": 128, "Max": 65536, "Inc": 128}&lt;/c&gt;&lt;c&gt;["hex", "number"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>58</v>
-      </c>
-      <c r="D39" t="s">
-        <v>66</v>
-      </c>
-      <c r="F39" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" t="s">
+        <v>58</v>
+      </c>
+      <c r="E39" t="s">
+        <v>65</v>
+      </c>
+      <c r="G39" t="s">
         <v>59</v>
-      </c>
-      <c r="G39" t="s">
-        <v>41</v>
       </c>
       <c r="H39" t="s">
         <v>41</v>
       </c>
       <c r="I39" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="J39" t="s">
-        <v>51</v>
-      </c>
-      <c r="K39" t="str">
-        <f>_xlfn.CONCAT(I39,_xlfn.TEXTJOIN(_xlfn.CONCAT(J39,I39),FALSE,A39:H39),J39)</f>
-        <v>&lt;c&gt;TDES-CTR&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;{"Min": 1, "Max": 64, "Inc": any}&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;</v>
+        <v>50</v>
+      </c>
+      <c r="K39" t="s">
+        <v>51</v>
+      </c>
+      <c r="L39" t="str">
+        <f>_xlfn.CONCAT(J39,_xlfn.TEXTJOIN(_xlfn.CONCAT(K39,J39),FALSE,A39:I39),K39)</f>
+        <v>&lt;c&gt;TDES-CTR&lt;/c&gt;&lt;c&gt;"1.0.0"&lt;/c&gt;&lt;c&gt;["encrypt", "decrypt"]&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;{"Min": 1, "Max": 64, "Inc": any}&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;[1, 2] Note: 2 is only available for decrypt operations&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;</v>
       </c>
     </row>
   </sheetData>
@@ -2145,7 +2247,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6147422C-C6BB-4B90-9E5E-89D3819A0EF0}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
@@ -2163,16 +2265,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>79</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>80</v>
-      </c>
-      <c r="E1" t="s">
-        <v>81</v>
       </c>
       <c r="F1" t="s">
         <v>48</v>
@@ -2187,7 +2289,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
         <v>41</v>
@@ -2202,13 +2304,13 @@
         <v>51</v>
       </c>
       <c r="H2" t="str">
-        <f>_xlfn.CONCAT(F2,_xlfn.TEXTJOIN(_xlfn.CONCAT(G2,F2),FALSE,A2:E2),G2)</f>
+        <f t="shared" ref="H2:H7" si="0">_xlfn.CONCAT(F2,_xlfn.TEXTJOIN(_xlfn.CONCAT(G2,F2),FALSE,A2:E2),G2)</f>
         <v>&lt;c&gt;SHA3-224&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s">
         <v>41</v>
@@ -2223,13 +2325,13 @@
         <v>51</v>
       </c>
       <c r="H3" t="str">
-        <f>_xlfn.CONCAT(F3,_xlfn.TEXTJOIN(_xlfn.CONCAT(G3,F3),FALSE,A3:E3),G3)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;SHA3-256&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4" t="s">
         <v>41</v>
@@ -2244,13 +2346,13 @@
         <v>51</v>
       </c>
       <c r="H4" t="str">
-        <f>_xlfn.CONCAT(F4,_xlfn.TEXTJOIN(_xlfn.CONCAT(G4,F4),FALSE,A4:E4),G4)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;SHA3-384&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B5" t="s">
         <v>41</v>
@@ -2265,13 +2367,13 @@
         <v>51</v>
       </c>
       <c r="H5" t="str">
-        <f>_xlfn.CONCAT(F5,_xlfn.TEXTJOIN(_xlfn.CONCAT(G5,F5),FALSE,A5:E5),G5)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;SHA3-512&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;&lt;/c&gt;&lt;c&gt;&lt;/c&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" t="s">
         <v>41</v>
@@ -2280,7 +2382,7 @@
         <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E6" t="s">
         <v>41</v>
@@ -2292,13 +2394,13 @@
         <v>51</v>
       </c>
       <c r="H6" t="str">
-        <f>_xlfn.CONCAT(F6,_xlfn.TEXTJOIN(_xlfn.CONCAT(G6,F6),FALSE,A6:E6),G6)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;SHAKE-128&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;{"Min": 16, "Max": 65536, "Inc": any}&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B7" t="s">
         <v>41</v>
@@ -2307,7 +2409,7 @@
         <v>41</v>
       </c>
       <c r="D7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E7" t="s">
         <v>41</v>
@@ -2319,7 +2421,7 @@
         <v>51</v>
       </c>
       <c r="H7" t="str">
-        <f>_xlfn.CONCAT(F7,_xlfn.TEXTJOIN(_xlfn.CONCAT(G7,F7),FALSE,A7:E7),G7)</f>
+        <f t="shared" si="0"/>
         <v>&lt;c&gt;SHAKE-256&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;&lt;c&gt;{"Min": 16, "Max": 65536, "Inc": any}&lt;/c&gt;&lt;c&gt;true, false&lt;/c&gt;</v>
       </c>
     </row>

</xml_diff>